<commit_message>
add latest official to spreadsheet
</commit_message>
<xml_diff>
--- a/output/ukraine_refugee_cost_estimates.xlsx
+++ b/output/ukraine_refugee_cost_estimates.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,17 +448,22 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>cost22</t>
+          <t>latest_reported_idrc</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>cost23</t>
+          <t>additional_cost_2022</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>cost24</t>
+          <t>additional_cost_2023</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>additional_cost_2024</t>
         </is>
       </c>
     </row>
@@ -472,12 +477,15 @@
         <v>93579</v>
       </c>
       <c r="C2" t="n">
+        <v>63.12</v>
+      </c>
+      <c r="D2" t="n">
         <v>129797392.8333333</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>94061333.59999999</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>468852.3666666665</v>
       </c>
     </row>
@@ -491,12 +499,15 @@
         <v>68304</v>
       </c>
       <c r="C3" t="n">
+        <v>250.67</v>
+      </c>
+      <c r="D3" t="n">
         <v>396528274.1166667</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>319975671.5333334</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>2320519.949999999</v>
       </c>
     </row>
@@ -510,12 +521,15 @@
         <v>492391</v>
       </c>
       <c r="C4" t="n">
+        <v>463.6</v>
+      </c>
+      <c r="D4" t="n">
         <v>926834896.8</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>4918043229.6</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -529,12 +543,15 @@
         <v>80773</v>
       </c>
       <c r="C5" t="n">
+        <v>368.35</v>
+      </c>
+      <c r="D5" t="n">
         <v>1027898810.875</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>889155661.75</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>6594908.874999998</v>
       </c>
     </row>
@@ -548,12 +565,15 @@
         <v>490802</v>
       </c>
       <c r="C6" t="n">
+        <v>6.42</v>
+      </c>
+      <c r="D6" t="n">
         <v>1450143541</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>1015440861</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>5112865.999999998</v>
       </c>
     </row>
@@ -567,12 +587,15 @@
         <v>1055323</v>
       </c>
       <c r="C7" t="n">
+        <v>2732.06</v>
+      </c>
+      <c r="D7" t="n">
         <v>8706475641.508333</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>7289371666.391666</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -586,12 +609,15 @@
         <v>39756</v>
       </c>
       <c r="C8" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="D8" t="n">
         <v>467799205.3</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>335415116.3</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -605,12 +631,15 @@
         <v>167726</v>
       </c>
       <c r="C9" t="n">
+        <v>232.08</v>
+      </c>
+      <c r="D9" t="n">
         <v>305259586.75</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>229639779.95</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>1790288.099999999</v>
       </c>
     </row>
@@ -624,12 +653,15 @@
         <v>47111</v>
       </c>
       <c r="C10" t="n">
+        <v>68.77</v>
+      </c>
+      <c r="D10" t="n">
         <v>426114124.325</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>402723831.975</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -643,12 +675,15 @@
         <v>118994</v>
       </c>
       <c r="C11" t="n">
+        <v>1156.48</v>
+      </c>
+      <c r="D11" t="n">
         <v>467716196.575</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>327532604.825</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -662,12 +697,15 @@
         <v>162700</v>
       </c>
       <c r="C12" t="n">
+        <v>1447.37</v>
+      </c>
+      <c r="D12" t="n">
         <v>1454658669.166667</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>1367324020.833333</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>10445340</v>
       </c>
     </row>
@@ -681,12 +719,15 @@
         <v>20955</v>
       </c>
       <c r="C13" t="n">
+        <v>36.55</v>
+      </c>
+      <c r="D13" t="n">
         <v>12354824.99166667</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>10211614.50833333</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -700,12 +741,15 @@
         <v>34248</v>
       </c>
       <c r="C14" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="D14" t="n">
         <v>142191881</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>105471180.2</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>484247.5999999999</v>
       </c>
     </row>
@@ -719,12 +763,15 @@
         <v>75260</v>
       </c>
       <c r="C15" t="n">
+        <v>50.29</v>
+      </c>
+      <c r="D15" t="n">
         <v>437023707.1666666</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>524745761.1666666</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>4418411.666666665</v>
       </c>
     </row>
@@ -738,12 +785,15 @@
         <v>2239</v>
       </c>
       <c r="C16" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="D16" t="n">
         <v>6001454.1</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>6840778.199999999</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -757,12 +807,15 @@
         <v>175143</v>
       </c>
       <c r="C17" t="n">
+        <v>556.1</v>
+      </c>
+      <c r="D17" t="n">
         <v>1465441727.583333</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>1164312903.116667</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -776,12 +829,15 @@
         <v>1800</v>
       </c>
       <c r="C18" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="D18" t="n">
         <v>23772.5</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>22487.5</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -794,13 +850,14 @@
       <c r="B19" t="n">
         <v>6756</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="n">
         <v>556804.9666666667</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>327555.4333333333</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>0</v>
       </c>
     </row>
@@ -814,12 +871,15 @@
         <v>89730</v>
       </c>
       <c r="C20" t="n">
+        <v>407.65</v>
+      </c>
+      <c r="D20" t="n">
         <v>1196589472</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>937811472</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>8997511.999999996</v>
       </c>
     </row>
@@ -833,12 +893,15 @@
         <v>39931</v>
       </c>
       <c r="C21" t="n">
+        <v>52.25</v>
+      </c>
+      <c r="D21" t="n">
         <v>388583552.2500001</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>473907827.7</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>5444842.949999998</v>
       </c>
     </row>
@@ -852,12 +915,15 @@
         <v>4000</v>
       </c>
       <c r="C22" t="n">
+        <v>11.67</v>
+      </c>
+      <c r="D22" t="n">
         <v>76276333.33333334</v>
       </c>
-      <c r="D22" t="n">
+      <c r="E22" t="n">
         <v>15255266.66666666</v>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -871,12 +937,15 @@
         <v>1563386</v>
       </c>
       <c r="C23" t="n">
+        <v>16.88</v>
+      </c>
+      <c r="D23" t="n">
         <v>1623782777.65</v>
       </c>
-      <c r="D23" t="n">
+      <c r="E23" t="n">
         <v>1144817489.75</v>
       </c>
-      <c r="E23" t="n">
+      <c r="F23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -890,12 +959,15 @@
         <v>58043</v>
       </c>
       <c r="C24" t="n">
+        <v>10.08</v>
+      </c>
+      <c r="D24" t="n">
         <v>219824366.3</v>
       </c>
-      <c r="D24" t="n">
+      <c r="E24" t="n">
         <v>154601379.35</v>
       </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
         <v>613294.5499999997</v>
       </c>
     </row>
@@ -909,12 +981,15 @@
         <v>109828</v>
       </c>
       <c r="C25" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="D25" t="n">
         <v>231189205.125</v>
       </c>
-      <c r="D25" t="n">
+      <c r="E25" t="n">
         <v>179747100.875</v>
       </c>
-      <c r="E25" t="n">
+      <c r="F25" t="n">
         <v>1281126.4</v>
       </c>
     </row>
@@ -928,12 +1003,15 @@
         <v>9081</v>
       </c>
       <c r="C26" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="D26" t="n">
         <v>3394028.733333333</v>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
         <v>2579453.066666666</v>
       </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -947,12 +1025,15 @@
         <v>50740</v>
       </c>
       <c r="C27" t="n">
+        <v>87.91</v>
+      </c>
+      <c r="D27" t="n">
         <v>268969632.75</v>
       </c>
-      <c r="D27" t="n">
+      <c r="E27" t="n">
         <v>180076659.75</v>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>154927.4999999999</v>
       </c>
     </row>
@@ -966,12 +1047,15 @@
         <v>85000</v>
       </c>
       <c r="C28" t="n">
+        <v>4745.18</v>
+      </c>
+      <c r="D28" t="n">
         <v>485675433.3333333</v>
       </c>
-      <c r="D28" t="n">
+      <c r="E28" t="n">
         <v>345514066.6666667</v>
       </c>
-      <c r="E28" t="n">
+      <c r="F28" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
year and actual cost
</commit_message>
<xml_diff>
--- a/output/ukraine_refugee_cost_estimates.xlsx
+++ b/output/ukraine_refugee_cost_estimates.xlsx
@@ -477,16 +477,16 @@
         <v>95753</v>
       </c>
       <c r="C2" t="n">
-        <v>63120000</v>
+        <v>58559136.85168231</v>
       </c>
       <c r="D2" t="n">
-        <v>130235970.7083333</v>
+        <v>120825497.2916667</v>
       </c>
       <c r="E2" t="n">
-        <v>97360129.86666667</v>
+        <v>90325169.33333333</v>
       </c>
       <c r="F2" t="n">
-        <v>2718590.325</v>
+        <v>2522152.875</v>
       </c>
     </row>
     <row r="3">
@@ -499,16 +499,16 @@
         <v>70613</v>
       </c>
       <c r="C3" t="n">
-        <v>250670000</v>
+        <v>238004283.1466135</v>
       </c>
       <c r="D3" t="n">
-        <v>395887733.95</v>
+        <v>375887809.2166666</v>
       </c>
       <c r="E3" t="n">
-        <v>333020573.375</v>
+        <v>316196646.2083333</v>
       </c>
       <c r="F3" t="n">
-        <v>13015422.375</v>
+        <v>12357893.875</v>
       </c>
     </row>
     <row r="4">
@@ -521,16 +521,16 @@
         <v>177958</v>
       </c>
       <c r="C4" t="n">
-        <v>463600000</v>
+        <v>483317981.6974695</v>
       </c>
       <c r="D4" t="n">
-        <v>701520971.7</v>
+        <v>731356400.6999999</v>
       </c>
       <c r="E4" t="n">
-        <v>1385939138.6</v>
+        <v>1444882620.6</v>
       </c>
       <c r="F4" t="n">
-        <v>33995003.49999999</v>
+        <v>35440798.49999999</v>
       </c>
     </row>
     <row r="5">
@@ -543,13 +543,13 @@
         <v>77450</v>
       </c>
       <c r="C5" t="n">
-        <v>368350000</v>
+        <v>363211408.4846383</v>
       </c>
       <c r="D5" t="n">
-        <v>1025688971.941666</v>
+        <v>1011381128.066666</v>
       </c>
       <c r="E5" t="n">
-        <v>814856063.0583333</v>
+        <v>803489231.9333333</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -565,16 +565,16 @@
         <v>504352</v>
       </c>
       <c r="C6" t="n">
-        <v>6420000</v>
+        <v>6480470.109048648</v>
       </c>
       <c r="D6" t="n">
-        <v>1432139176.416667</v>
+        <v>1445649651.6</v>
       </c>
       <c r="E6" t="n">
-        <v>1043257674.833333</v>
+        <v>1053099530.4</v>
       </c>
       <c r="F6" t="n">
-        <v>31989116.75</v>
+        <v>32290894.8</v>
       </c>
     </row>
     <row r="7">
@@ -587,16 +587,16 @@
         <v>1056628</v>
       </c>
       <c r="C7" t="n">
-        <v>2732060000</v>
+        <v>2567870947.881485</v>
       </c>
       <c r="D7" t="n">
-        <v>8720089113.083332</v>
+        <v>8195999177.849999</v>
       </c>
       <c r="E7" t="n">
-        <v>7232123398.083333</v>
+        <v>6797462348.85</v>
       </c>
       <c r="F7" t="n">
-        <v>88457156.8333333</v>
+        <v>83140754.09999998</v>
       </c>
     </row>
     <row r="8">
@@ -609,16 +609,16 @@
         <v>41821</v>
       </c>
       <c r="C8" t="n">
-        <v>63200000</v>
+        <v>60858884.68409418</v>
       </c>
       <c r="D8" t="n">
-        <v>473580821.5249999</v>
+        <v>456036846.2999999</v>
       </c>
       <c r="E8" t="n">
-        <v>369836570.6</v>
+        <v>356135839.1999999</v>
       </c>
       <c r="F8" t="n">
-        <v>11960067.175</v>
+        <v>11517002.1</v>
       </c>
     </row>
     <row r="9">
@@ -631,16 +631,16 @@
         <v>173169</v>
       </c>
       <c r="C9" t="n">
-        <v>232080000</v>
+        <v>212595686.1506533</v>
       </c>
       <c r="D9" t="n">
-        <v>307320217.7499999</v>
+        <v>281514630.4583333</v>
       </c>
       <c r="E9" t="n">
-        <v>240735758.9</v>
+        <v>220521248.8166667</v>
       </c>
       <c r="F9" t="n">
-        <v>9790639.950000001</v>
+        <v>8968522.825000001</v>
       </c>
     </row>
     <row r="10">
@@ -653,13 +653,13 @@
         <v>47111</v>
       </c>
       <c r="C10" t="n">
-        <v>68770000</v>
+        <v>64843054.67945981</v>
       </c>
       <c r="D10" t="n">
-        <v>426145610.6499999</v>
+        <v>401811525.475</v>
       </c>
       <c r="E10" t="n">
-        <v>402753589.9499999</v>
+        <v>379755253.4250001</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -675,13 +675,13 @@
         <v>118994</v>
       </c>
       <c r="C11" t="n">
-        <v>1156480000</v>
+        <v>1052522864.031498</v>
       </c>
       <c r="D11" t="n">
-        <v>470277644.5249999</v>
+        <v>427999756.3666667</v>
       </c>
       <c r="E11" t="n">
-        <v>329326337.275</v>
+        <v>299719950.0333334</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -697,16 +697,16 @@
         <v>199900</v>
       </c>
       <c r="C12" t="n">
-        <v>1447370000</v>
+        <v>1359976138.191323</v>
       </c>
       <c r="D12" t="n">
-        <v>1451491808.333333</v>
+        <v>1363847472.5</v>
       </c>
       <c r="E12" t="n">
-        <v>1828152991.666667</v>
+        <v>1717765007.5</v>
       </c>
       <c r="F12" t="n">
-        <v>192818100</v>
+        <v>181175310</v>
       </c>
     </row>
     <row r="13">
@@ -719,16 +719,16 @@
         <v>22704</v>
       </c>
       <c r="C13" t="n">
-        <v>36550000</v>
+        <v>35077534.88405661</v>
       </c>
       <c r="D13" t="n">
-        <v>12296314.81666666</v>
+        <v>11800699.21666666</v>
       </c>
       <c r="E13" t="n">
-        <v>11725402.68333333</v>
+        <v>11252798.28333333</v>
       </c>
       <c r="F13" t="n">
-        <v>312429.6999999998</v>
+        <v>299836.8999999998</v>
       </c>
     </row>
     <row r="14">
@@ -741,16 +741,16 @@
         <v>34248</v>
       </c>
       <c r="C14" t="n">
-        <v>1380000</v>
+        <v>1276285.374746241</v>
       </c>
       <c r="D14" t="n">
-        <v>141330361.7916667</v>
+        <v>130707574.8333333</v>
       </c>
       <c r="E14" t="n">
-        <v>103869518.9583333</v>
+        <v>96062394.16666666</v>
       </c>
       <c r="F14" t="n">
-        <v>1443940.85</v>
+        <v>1335410.2</v>
       </c>
     </row>
     <row r="15">
@@ -763,16 +763,16 @@
         <v>78462</v>
       </c>
       <c r="C15" t="n">
-        <v>50290000</v>
+        <v>47432854.05086241</v>
       </c>
       <c r="D15" t="n">
-        <v>441813334.4916667</v>
+        <v>416711193.8416666</v>
       </c>
       <c r="E15" t="n">
-        <v>560661453.5083333</v>
+        <v>528806818.1583333</v>
       </c>
       <c r="F15" t="n">
-        <v>15859971.39999999</v>
+        <v>14958868.59999999</v>
       </c>
     </row>
     <row r="16">
@@ -785,16 +785,16 @@
         <v>2674</v>
       </c>
       <c r="C16" t="n">
-        <v>4330000</v>
+        <v>4314709.876317098</v>
       </c>
       <c r="D16" t="n">
-        <v>6098972.366666666</v>
+        <v>6077417.899999999</v>
       </c>
       <c r="E16" t="n">
-        <v>9276208.608333332</v>
+        <v>9243425.425000001</v>
       </c>
       <c r="F16" t="n">
-        <v>211297.6249999999</v>
+        <v>210550.8749999999</v>
       </c>
     </row>
     <row r="17">
@@ -807,16 +807,16 @@
         <v>178519</v>
       </c>
       <c r="C17" t="n">
-        <v>556100000</v>
+        <v>510450554.9054651</v>
       </c>
       <c r="D17" t="n">
-        <v>1459536978</v>
+        <v>1339734000.916667</v>
       </c>
       <c r="E17" t="n">
-        <v>1196927744.4</v>
+        <v>1098680485.65</v>
       </c>
       <c r="F17" t="n">
-        <v>13179811.2</v>
+        <v>12097974.53333333</v>
       </c>
     </row>
     <row r="18">
@@ -829,13 +829,13 @@
         <v>1800</v>
       </c>
       <c r="C18" t="n">
-        <v>270000</v>
+        <v>224926.0855395237</v>
       </c>
       <c r="D18" t="n">
-        <v>23680</v>
+        <v>19795</v>
       </c>
       <c r="E18" t="n">
-        <v>22400</v>
+        <v>18725</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -851,16 +851,16 @@
         <v>76540</v>
       </c>
       <c r="C19" t="n">
-        <v>1910000</v>
+        <v>1966967.651507459</v>
       </c>
       <c r="D19" t="n">
-        <v>157762188.225</v>
+        <v>162465020.075</v>
       </c>
       <c r="E19" t="n">
-        <v>116636779.8</v>
+        <v>120113678.6</v>
       </c>
       <c r="F19" t="n">
-        <v>3418269.975</v>
+        <v>3520167.325</v>
       </c>
     </row>
     <row r="20">
@@ -874,10 +874,10 @@
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="n">
-        <v>566163.0333333332</v>
+        <v>533409.7999999999</v>
       </c>
       <c r="E20" t="n">
-        <v>333060.5666666667</v>
+        <v>313792.6</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -893,16 +893,16 @@
         <v>89730</v>
       </c>
       <c r="C21" t="n">
-        <v>407650000</v>
+        <v>383424781.3742747</v>
       </c>
       <c r="D21" t="n">
-        <v>1195111718.666667</v>
+        <v>1124089390.666667</v>
       </c>
       <c r="E21" t="n">
-        <v>936653302</v>
+        <v>880990474</v>
       </c>
       <c r="F21" t="n">
-        <v>8986400.33333333</v>
+        <v>8452362.33333333</v>
       </c>
     </row>
     <row r="22">
@@ -915,16 +915,16 @@
         <v>45238</v>
       </c>
       <c r="C22" t="n">
-        <v>52250000</v>
+        <v>56366852.26050603</v>
       </c>
       <c r="D22" t="n">
-        <v>393768027.25</v>
+        <v>424794428.5</v>
       </c>
       <c r="E22" t="n">
-        <v>556864310.2750001</v>
+        <v>600741655.1500001</v>
       </c>
       <c r="F22" t="n">
-        <v>45775326.675</v>
+        <v>49382129.55</v>
       </c>
     </row>
     <row r="23">
@@ -937,13 +937,13 @@
         <v>4000</v>
       </c>
       <c r="C23" t="n">
-        <v>11670000</v>
+        <v>11052205.68546864</v>
       </c>
       <c r="D23" t="n">
-        <v>75920000</v>
+        <v>71900666.66666667</v>
       </c>
       <c r="E23" t="n">
-        <v>15183999.99999999</v>
+        <v>14380133.33333333</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
@@ -959,16 +959,16 @@
         <v>1583563</v>
       </c>
       <c r="C24" t="n">
-        <v>16880000</v>
+        <v>16303317.58315022</v>
       </c>
       <c r="D24" t="n">
-        <v>1633777261.966666</v>
+        <v>1577936519.316667</v>
       </c>
       <c r="E24" t="n">
-        <v>1178827446.783333</v>
+        <v>1138536397.558333</v>
       </c>
       <c r="F24" t="n">
-        <v>8987844.65</v>
+        <v>8680649.825000001</v>
       </c>
     </row>
     <row r="25">
@@ -981,16 +981,16 @@
         <v>58242</v>
       </c>
       <c r="C25" t="n">
-        <v>11050000</v>
+        <v>10345677.54923651</v>
       </c>
       <c r="D25" t="n">
-        <v>226244160.45</v>
+        <v>211822587.9</v>
       </c>
       <c r="E25" t="n">
-        <v>160329477.6</v>
+        <v>150109531.2</v>
       </c>
       <c r="F25" t="n">
-        <v>741486.1499999998</v>
+        <v>694221.2999999997</v>
       </c>
     </row>
     <row r="26">
@@ -1003,16 +1003,16 @@
         <v>113024</v>
       </c>
       <c r="C26" t="n">
-        <v>1210000</v>
+        <v>1154865.353723471</v>
       </c>
       <c r="D26" t="n">
-        <v>231441749.75</v>
+        <v>220896471.7499999</v>
       </c>
       <c r="E26" t="n">
-        <v>186384887.65</v>
+        <v>177892554.45</v>
       </c>
       <c r="F26" t="n">
-        <v>6849740.2</v>
+        <v>6537642.6</v>
       </c>
     </row>
     <row r="27">
@@ -1025,16 +1025,16 @@
         <v>9222</v>
       </c>
       <c r="C27" t="n">
-        <v>2330000</v>
+        <v>2209267.842568598</v>
       </c>
       <c r="D27" t="n">
-        <v>3399188.4</v>
+        <v>3223243.766666667</v>
       </c>
       <c r="E27" t="n">
-        <v>2653042.5</v>
+        <v>2515718.958333333</v>
       </c>
       <c r="F27" t="n">
-        <v>23222.7</v>
+        <v>22020.675</v>
       </c>
     </row>
     <row r="28">
@@ -1047,16 +1047,16 @@
         <v>53957</v>
       </c>
       <c r="C28" t="n">
-        <v>87910000</v>
+        <v>79263094.67844568</v>
       </c>
       <c r="D28" t="n">
-        <v>269881085.25</v>
+        <v>243333512.1</v>
       </c>
       <c r="E28" t="n">
-        <v>201808435.5</v>
+        <v>181957010.2</v>
       </c>
       <c r="F28" t="n">
-        <v>7610510.25</v>
+        <v>6861882.1</v>
       </c>
     </row>
     <row r="29">
@@ -1069,13 +1069,13 @@
         <v>85000</v>
       </c>
       <c r="C29" t="n">
-        <v>4745180000</v>
+        <v>5072989206.702785</v>
       </c>
       <c r="D29" t="n">
-        <v>487085966.6666666</v>
+        <v>520735133.3333333</v>
       </c>
       <c r="E29" t="n">
-        <v>346517533.3333334</v>
+        <v>370455866.6666666</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
@@ -1119,7 +1119,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2405.3</v>
+        <v>2231.5</v>
       </c>
     </row>
     <row r="3">
@@ -1129,7 +1129,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10506.9</v>
+        <v>9976.1</v>
       </c>
     </row>
     <row r="4">
@@ -1139,7 +1139,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>11921.1</v>
+        <v>12428.1</v>
       </c>
     </row>
     <row r="5">
@@ -1149,7 +1149,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>23764.3</v>
+        <v>23432.8</v>
       </c>
     </row>
     <row r="6">
@@ -1159,7 +1159,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4971.5</v>
+        <v>5018.4</v>
       </c>
     </row>
     <row r="7">
@@ -1169,7 +1169,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>15181</v>
+        <v>14268.6</v>
       </c>
     </row>
     <row r="8">
@@ -1179,7 +1179,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>20453.3</v>
+        <v>19695.6</v>
       </c>
     </row>
     <row r="9">
@@ -1189,7 +1189,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3221.4</v>
+        <v>2950.9</v>
       </c>
     </row>
     <row r="10">
@@ -1199,7 +1199,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17594.6</v>
+        <v>16589.9</v>
       </c>
     </row>
     <row r="11">
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6719.7</v>
+        <v>6115.6</v>
       </c>
     </row>
     <row r="12">
@@ -1219,7 +1219,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17371</v>
+        <v>16322.1</v>
       </c>
     </row>
     <row r="13">
@@ -1229,7 +1229,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1071.8</v>
+        <v>1028.6</v>
       </c>
     </row>
     <row r="14">
@@ -1239,7 +1239,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>7201.7</v>
+        <v>6660.4</v>
       </c>
     </row>
     <row r="15">
@@ -1249,7 +1249,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>12978.7</v>
+        <v>12241.3</v>
       </c>
     </row>
     <row r="16">
@@ -1259,7 +1259,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>5828.9</v>
+        <v>5808.3</v>
       </c>
     </row>
     <row r="17">
@@ -1269,7 +1269,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>14954.4</v>
+        <v>13726.9</v>
       </c>
     </row>
     <row r="18">
@@ -1279,7 +1279,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>25.6</v>
+        <v>21.4</v>
       </c>
     </row>
     <row r="19">
@@ -1289,7 +1289,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>130.4</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20">
@@ -1299,7 +1299,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>3629.7</v>
+        <v>3737.9</v>
       </c>
     </row>
     <row r="21">
@@ -1309,7 +1309,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>133.1</v>
+        <v>125.4</v>
       </c>
     </row>
     <row r="22">
@@ -1319,7 +1319,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>23857.7</v>
+        <v>22439.9</v>
       </c>
     </row>
     <row r="23">
@@ -1329,7 +1329,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>22025.9</v>
+        <v>23761.4</v>
       </c>
     </row>
     <row r="24">
@@ -1339,7 +1339,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>22776</v>
+        <v>21570.2</v>
       </c>
     </row>
     <row r="25">
@@ -1349,7 +1349,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1781.8</v>
+        <v>1720.9</v>
       </c>
     </row>
     <row r="26">
@@ -1359,7 +1359,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>6650.1</v>
+        <v>6226.2</v>
       </c>
     </row>
     <row r="27">
@@ -1369,7 +1369,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>3757.4</v>
+        <v>3586.2</v>
       </c>
     </row>
     <row r="28">
@@ -1379,7 +1379,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>658.8</v>
+        <v>624.7</v>
       </c>
     </row>
     <row r="29">
@@ -1389,7 +1389,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>8883</v>
+        <v>8009.2</v>
       </c>
     </row>
     <row r="30">
@@ -1399,7 +1399,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>9807.1</v>
+        <v>10484.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>